<commit_message>
Many fixes: legend issues, some of the building energy concerns
</commit_message>
<xml_diff>
--- a/Resources/Catégories des bâtiments.xlsx
+++ b/Resources/Catégories des bâtiments.xlsx
@@ -628,7 +628,7 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -823,9 +823,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>30</xdr:col>
-      <xdr:colOff>131040</xdr:colOff>
+      <xdr:colOff>130680</xdr:colOff>
       <xdr:row>70</xdr:row>
-      <xdr:rowOff>108360</xdr:rowOff>
+      <xdr:rowOff>108000</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -838,8 +838,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="11553840" y="8749800"/>
-          <a:ext cx="4390560" cy="3626640"/>
+          <a:off x="11570400" y="8749800"/>
+          <a:ext cx="4388760" cy="3626280"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -860,9 +860,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>17</xdr:col>
-      <xdr:colOff>82800</xdr:colOff>
+      <xdr:colOff>82440</xdr:colOff>
       <xdr:row>54</xdr:row>
-      <xdr:rowOff>1440</xdr:rowOff>
+      <xdr:rowOff>1080</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -875,8 +875,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9668880" y="8370000"/>
-          <a:ext cx="1967760" cy="1095480"/>
+          <a:off x="9684000" y="8370000"/>
+          <a:ext cx="1968840" cy="1095120"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -898,18 +898,18 @@
   </sheetPr>
   <dimension ref="A2:AQ49"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="M22" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="AM23" activeCellId="0" sqref="AM23"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="L12" activeCellId="0" sqref="C12:L12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.70703125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.72265625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="14" style="0" width="3.97"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="1" width="12.85"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="17" style="0" width="3.97"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="1" width="5.9"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="1" width="5.89"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="20" style="0" width="3.97"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="22" style="1" width="6.24"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="22" style="1" width="6.23"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="24" min="23" style="0" width="3.97"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="25" min="25" style="1" width="6.42"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="27" min="26" style="0" width="3.97"/>
@@ -1572,34 +1572,34 @@
         <v>63</v>
       </c>
       <c r="C7" s="2" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D7" s="2" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E7" s="2" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F7" s="2" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="G7" s="2" t="n">
-        <v>2</v>
+        <v>0.666666666666667</v>
       </c>
       <c r="H7" s="2" t="n">
-        <v>2</v>
+        <v>0.666666666666667</v>
       </c>
       <c r="I7" s="2" t="n">
-        <v>1.5</v>
+        <v>0.5</v>
       </c>
       <c r="J7" s="2" t="n">
-        <v>1.5</v>
+        <v>0.5</v>
       </c>
       <c r="K7" s="2" t="n">
-        <v>1.3</v>
+        <v>0.433333333333333</v>
       </c>
       <c r="L7" s="2" t="n">
-        <v>0.6</v>
+        <v>0.2</v>
       </c>
       <c r="P7" s="1" t="str">
         <f aca="false">CONCATENATE(TEXT(P3,"##.###"),",",TEXT(S3,"##.###"),",",TEXT(V3,"##.###"),",",TEXT(Y3,"##.###"),",",TEXT(AB3,"##.###"),",",TEXT(AE3,"##.###"),",",TEXT(AH3,"##.###"),",",TEXT(AK3,"##.###"),",",TEXT(AN3,"##.###"),",",TEXT(AQ3,"##.###"))</f>
@@ -1707,7 +1707,7 @@
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="P11" s="1" t="str">
         <f aca="false">CONCATENATE(TEXT(C7,"##.###"),",",TEXT(D7,"##.###"),",",TEXT(E7,"##.###"),",",TEXT(F7,"##.###"),",",TEXT(G7,"##.###"),",",TEXT(H7,"##.###"),",",TEXT(I7,"##.###"),",",TEXT(J7,"##.###"),",",TEXT(K7,"##.###"),",",TEXT(L7,"##.###"))</f>
-        <v>3,3,3,3,2,2,1.5,1.5,1.3,.6</v>
+        <v>1,1,1,1,.667,.667,.5,.5,.433,.2</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3632,10 +3632,10 @@
   <dimension ref="B3:E30"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G25" activeCellId="0" sqref="G25"/>
+      <selection pane="topLeft" activeCell="G25" activeCellId="1" sqref="C12:L12 G25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.70703125" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.72265625" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="33.56"/>
   </cols>

</xml_diff>